<commit_message>
include font-awesome and complete personal-home
</commit_message>
<xml_diff>
--- a/项目规划.xlsx
+++ b/项目规划.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15">
   <si>
     <t>编号</t>
   </si>
@@ -31,21 +31,12 @@
     <t>优先级</t>
   </si>
   <si>
-    <t>注册登录</t>
-  </si>
-  <si>
-    <t>出完整的图，并设为1200px宽</t>
-  </si>
-  <si>
-    <t>个人主页</t>
+    <t>具体图片</t>
   </si>
   <si>
     <t>设计</t>
   </si>
   <si>
-    <t>具体图片</t>
-  </si>
-  <si>
     <t>广场页面</t>
   </si>
   <si>
@@ -59,6 +50,18 @@
   </si>
   <si>
     <t>MVC构架</t>
+  </si>
+  <si>
+    <t>登录注册</t>
+  </si>
+  <si>
+    <t>后台实现</t>
+  </si>
+  <si>
+    <t>数据库</t>
+  </si>
+  <si>
+    <t>数据库构架</t>
   </si>
 </sst>
 </file>
@@ -66,29 +69,22 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="宋体"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="宋体"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -128,19 +124,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -467,11 +463,11 @@
         </a:custGeom>
         <a:gradFill rotWithShape="0">
           <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="BBD5F0"/>
+            </a:gs>
             <a:gs pos="100000">
               <a:srgbClr val="9CBEE0"/>
-            </a:gs>
-            <a:gs pos="0">
-              <a:srgbClr val="BBD5F0"/>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
@@ -495,10 +491,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="3"/>
@@ -544,7 +540,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
@@ -555,10 +551,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -569,13 +565,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -583,10 +579,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -600,10 +596,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -611,10 +607,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
@@ -624,14 +620,14 @@
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>8</v>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -639,40 +635,12 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="2">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new planning ,please add your mission and the complete date by yourself
</commit_message>
<xml_diff>
--- a/项目规划.xlsx
+++ b/项目规划.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19800" windowHeight="7950"/>
+    <workbookView windowWidth="19830" windowHeight="8955"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,40 +28,41 @@
     <t>描述</t>
   </si>
   <si>
-    <t>优先级</t>
-  </si>
-  <si>
-    <t>登录注册</t>
-  </si>
-  <si>
-    <t>后台实现</t>
-  </si>
-  <si>
-    <t>数据库</t>
-  </si>
-  <si>
-    <t>数据库构架</t>
-  </si>
-  <si>
-    <t>上传图片</t>
-  </si>
-  <si>
-    <t>加载主页图片</t>
-  </si>
-  <si>
-    <t>修改信息</t>
-  </si>
-  <si>
-    <t>加载具体图片</t>
-  </si>
-  <si>
-    <t>关注功能</t>
-  </si>
-  <si>
-    <t>评论点赞功能</t>
-  </si>
-  <si>
-    <t>提醒功能</t>
+    <t>截止日期</t>
+  </si>
+  <si>
+    <t>是否完成</t>
+  </si>
+  <si>
+    <t>个人设置</t>
+  </si>
+  <si>
+    <t>个人设置前端实现</t>
+  </si>
+  <si>
+    <t>成员</t>
+  </si>
+  <si>
+    <t>分工</t>
+  </si>
+  <si>
+    <t>戴政</t>
+  </si>
+  <si>
+    <t>网页前端以
+及ajax-java后台交互</t>
+  </si>
+  <si>
+    <t>梁世宇</t>
+  </si>
+  <si>
+    <t>郝俊楠</t>
+  </si>
+  <si>
+    <t>胡长铼</t>
+  </si>
+  <si>
+    <t>张永斌</t>
   </si>
 </sst>
 </file>
@@ -140,7 +141,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -149,6 +150,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -491,21 +498,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="12.375" style="1" customWidth="1"/>
     <col min="3" max="3" width="40.125" style="1" customWidth="1"/>
-    <col min="4" max="16383" width="9" style="1"/>
+    <col min="4" max="6" width="9" style="1"/>
+    <col min="7" max="7" width="16.875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9" style="1"/>
+    <col min="9" max="9" width="22.125" style="1" customWidth="1"/>
+    <col min="10" max="16383" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -518,132 +529,234 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>42019</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="2">
-        <v>4</v>
-      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="24" spans="6:7">
+      <c r="F24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" ht="51" customHeight="1" spans="6:7">
+      <c r="F25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="6:7">
+      <c r="F26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="6:7">
+      <c r="F27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="6:7">
+      <c r="F28" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="6:7">
+      <c r="F29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>